<commit_message>
Added the 10 and 101 long and lat
</commit_message>
<xml_diff>
--- a/Assets/Offramp Coordinate Info/Offramp coordinates.xlsx
+++ b/Assets/Offramp Coordinate Info/Offramp coordinates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="22320" yWindow="0" windowWidth="9660" windowHeight="15780" tabRatio="500"/>
+    <workbookView xWindow="9360" yWindow="0" windowWidth="26580" windowHeight="15780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="140">
   <si>
     <t>Imperial Highway west</t>
   </si>
@@ -439,9 +439,6 @@
   </si>
   <si>
     <t>Longitude</t>
-  </si>
-  <si>
-    <t> -118.140428</t>
   </si>
 </sst>
 </file>
@@ -455,11 +452,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Courier"/>
     </font>
     <font>
       <u/>
@@ -478,18 +470,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -501,21 +505,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -847,155 +865,221 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="33.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1">
+      <c r="A1" s="1">
         <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="C3" s="2">
+        <v>33.931432000000001</v>
+      </c>
+      <c r="D3" s="2">
+        <v>-118.40397400000001</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="C4" s="2">
+        <v>33.931361000000003</v>
+      </c>
+      <c r="D4" s="2">
+        <v>-118.396164</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="C5" s="2">
+        <v>33.931165</v>
+      </c>
+      <c r="D5" s="2">
+        <v>-118.387473</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="C6" s="2">
+        <v>33.930008000000001</v>
+      </c>
+      <c r="D6" s="2">
+        <v>-118.370007</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="C7" s="2">
+        <v>33.930204000000003</v>
+      </c>
+      <c r="D7" s="2">
+        <v>-118.368419</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="C8" s="2">
+        <v>33.933729</v>
+      </c>
+      <c r="D8" s="2">
+        <v>-118.352605</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="C9" s="2">
+        <v>33.929989999999997</v>
+      </c>
+      <c r="D9" s="3">
+        <v>-118.34385</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="C10" s="2">
+        <v>33.925237000000003</v>
+      </c>
+      <c r="D10" s="2">
+        <v>-118.32658000000001</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="C11" s="2">
+        <v>33.928797000000003</v>
+      </c>
+      <c r="D11" s="2">
+        <v>-118.29173299999999</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="C12" s="2">
+        <v>33.928797000000003</v>
+      </c>
+      <c r="D12" s="2">
+        <v>-118.28066</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="C13" s="2">
+        <v>33.928387999999998</v>
+      </c>
+      <c r="D13" s="3">
+        <v>-118.254329</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="C14" s="2">
+        <v>33.928387999999998</v>
+      </c>
+      <c r="D14" s="2">
+        <v>-118.209976</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="C15" s="2">
+        <v>33.924934</v>
+      </c>
+      <c r="D15" s="2">
+        <v>-118.209976</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="C16" s="2">
+        <v>33.912897000000001</v>
+      </c>
+      <c r="D16" s="2">
+        <v>-118.180042</v>
+      </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="C17" s="2">
+        <v>33.911152000000001</v>
+      </c>
+      <c r="D17" s="2">
+        <v>-118.168927</v>
+      </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" ht="18">
-      <c r="A19" s="1" t="s">
+      <c r="C18" s="2">
+        <v>33.911971000000001</v>
+      </c>
+      <c r="D18" s="2">
+        <v>-118.159936</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="2">
         <v>33.91328</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="18">
-      <c r="A20" s="1" t="s">
+      <c r="D19" s="2">
+        <v>-118.140428</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="2">
@@ -1005,8 +1089,8 @@
         <v>-118.12542000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:4">
+      <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="2">
@@ -1016,8 +1100,8 @@
         <v>-118.104692</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="18">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:4">
+      <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="4">
@@ -1028,7 +1112,7 @@
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="3">
@@ -1039,637 +1123,878 @@
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29">
+      <c r="A29" s="1">
         <v>10</v>
       </c>
+      <c r="C29" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="C30" s="2">
+        <v>34.011422000000003</v>
+      </c>
+      <c r="D30" s="2">
+        <v>-118.49547</v>
+      </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C31" s="2">
+        <v>34.012774</v>
+      </c>
+      <c r="D31" s="2">
+        <v>-118.48933</v>
+      </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="1" t="s">
+      <c r="C32" s="2">
+        <v>34.014819000000003</v>
+      </c>
+      <c r="D32" s="1">
+        <v>-118.485857</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="1" t="s">
+      <c r="C33" s="2">
+        <v>34.023338000000003</v>
+      </c>
+      <c r="D33" s="2">
+        <v>-118.473798</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="1" t="s">
+      <c r="C34" s="2">
+        <v>34.024636000000001</v>
+      </c>
+      <c r="D34" s="2">
+        <v>-118.469356</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="1" t="s">
+      <c r="C35" s="2">
+        <v>34.027766</v>
+      </c>
+      <c r="D35" s="2">
+        <v>-118.455172</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="1" t="s">
+      <c r="C36" s="2">
+        <v>34.028281999999997</v>
+      </c>
+      <c r="D36" s="2">
+        <v>-118.44925000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="1" t="s">
+      <c r="C37" s="2">
+        <v>34.031376000000002</v>
+      </c>
+      <c r="D37" s="2">
+        <v>-118.43358600000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="1" t="s">
+      <c r="C38" s="2">
+        <v>34.031767000000002</v>
+      </c>
+      <c r="D38" s="2">
+        <v>-118.41702100000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="1" t="s">
+      <c r="C39" s="2">
+        <v>34.029668999999998</v>
+      </c>
+      <c r="D39" s="2">
+        <v>-118.40318000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="1" t="s">
+      <c r="C40" s="2">
+        <v>34.030664999999999</v>
+      </c>
+      <c r="D40" s="2">
+        <v>-118.391379</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="1" t="s">
+      <c r="C41" s="2">
+        <v>34.036942000000003</v>
+      </c>
+      <c r="D41" s="2">
+        <v>-118.377431</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="1" t="s">
+      <c r="C42" s="2">
+        <v>34.035359</v>
+      </c>
+      <c r="D42" s="2">
+        <v>-118.369535</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="1" t="s">
+      <c r="C43" s="2">
+        <v>34.034328000000002</v>
+      </c>
+      <c r="D43" s="2">
+        <v>-118.350137</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="1" t="s">
+      <c r="C44" s="2">
+        <v>34.035181999999999</v>
+      </c>
+      <c r="D44" s="2">
+        <v>-118.333786</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="1" t="s">
+      <c r="C45" s="2">
+        <v>34.036763999999998</v>
+      </c>
+      <c r="D45" s="2">
+        <v>-118.31771500000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="1" t="s">
+      <c r="B46" s="6"/>
+      <c r="C46" s="2">
+        <v>34.036977999999998</v>
+      </c>
+      <c r="D46" s="2">
+        <v>-118.30052999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="1" t="s">
+      <c r="C47" s="2">
+        <v>34.036977999999998</v>
+      </c>
+      <c r="D47" s="2">
+        <v>-118.291601</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="1" t="s">
+      <c r="C48" s="2">
+        <v>34.037154999999998</v>
+      </c>
+      <c r="D48" s="2">
+        <v>-118.28396499999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="1" t="s">
+      <c r="C49" s="2">
+        <v>34.038257999999999</v>
+      </c>
+      <c r="D49" s="2">
+        <v>-118.273966</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="1" t="s">
+      <c r="C50" s="2">
+        <v>34.034559000000002</v>
+      </c>
+      <c r="D50" s="2">
+        <v>-118.267117</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" s="1" t="s">
+      <c r="C51" s="2">
+        <v>34.031998999999999</v>
+      </c>
+      <c r="D51" s="2">
+        <v>-118.26239700000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="1" t="s">
+      <c r="C52" s="2">
+        <v>34.031252000000002</v>
+      </c>
+      <c r="D52" s="2">
+        <v>-118.259972</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="1" t="s">
+      <c r="C53" s="2">
+        <v>34.029651000000001</v>
+      </c>
+      <c r="D53" s="2">
+        <v>-118.256174</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="1" t="s">
+      <c r="C54" s="2">
+        <v>34.025970000000001</v>
+      </c>
+      <c r="D54" s="2">
+        <v>-118.249222</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="1" t="s">
+      <c r="C55" s="2">
+        <v>34.024619000000001</v>
+      </c>
+      <c r="D55" s="2">
+        <v>-118.239287</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" s="1" t="s">
+      <c r="C56" s="2">
+        <v>34.027979999999999</v>
+      </c>
+      <c r="D56" s="2">
+        <v>-118.231111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" s="1" t="s">
+      <c r="C57" s="2">
+        <v>34.029668999999998</v>
+      </c>
+      <c r="D57" s="2">
+        <v>-118.224653</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" s="1" t="s">
+      <c r="C58" s="2">
+        <v>34.033937000000002</v>
+      </c>
+      <c r="D58" s="2">
+        <v>-118.220799</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" s="1" t="s">
+      <c r="C59" s="2">
+        <v>34.043031999999997</v>
+      </c>
+      <c r="D59" s="2">
+        <v>-118.217259</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" s="1" t="s">
+      <c r="C60" s="2">
+        <v>34.049681999999997</v>
+      </c>
+      <c r="D60" s="1">
+        <v>-118.21423299999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" s="1" t="s">
+      <c r="C61" s="2">
+        <v>34.052002000000002</v>
+      </c>
+      <c r="D61" s="2">
+        <v>-118.21405300000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" s="1" t="s">
+      <c r="C62" s="2">
+        <v>34.056339000000001</v>
+      </c>
+      <c r="D62" s="2">
+        <v>-118.213751</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" s="1" t="s">
+      <c r="C63" s="2">
+        <v>34.055477000000003</v>
+      </c>
+      <c r="D63" s="2">
+        <v>-118.211658</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" s="1" t="s">
+      <c r="C64" s="2">
+        <v>34.055362000000002</v>
+      </c>
+      <c r="D64" s="2">
+        <v>-118.200599</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" s="1" t="s">
+      <c r="C65" s="2">
+        <v>34.055388000000001</v>
+      </c>
+      <c r="D65" s="2">
+        <v>-118.186156</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71">
+      <c r="C66" s="2">
+        <v>34.060578999999997</v>
+      </c>
+      <c r="D66" s="2">
+        <v>-118.173507</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="1">
         <v>101</v>
       </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" s="1" t="s">
+      <c r="C71" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
-      <c r="A73" s="1" t="s">
+    <row r="73" spans="1:4">
+      <c r="A73" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
-      <c r="A74" s="1" t="s">
+    <row r="74" spans="1:4">
+      <c r="A74" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:4">
+      <c r="A75" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:4">
+      <c r="A76" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
-      <c r="A77" s="1" t="s">
+    <row r="77" spans="1:4">
+      <c r="A77" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
-      <c r="A78" s="1" t="s">
+    <row r="78" spans="1:4">
+      <c r="A78" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
-      <c r="A79" s="1" t="s">
+    <row r="79" spans="1:4">
+      <c r="A79" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
-      <c r="A80" s="1" t="s">
+    <row r="80" spans="1:4">
+      <c r="A80" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="1" t="s">
+      <c r="A81" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83" s="1" t="s">
+      <c r="A83" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84" s="1" t="s">
+      <c r="A84" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85" s="1" t="s">
+      <c r="A85" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87" s="1" t="s">
+      <c r="A87" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88" s="1" t="s">
+      <c r="A88" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89" s="1" t="s">
+      <c r="A89" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="1" t="s">
+      <c r="A90" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="91" spans="1:1">
-      <c r="A91" s="1" t="s">
+      <c r="A91" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92" s="1" t="s">
+      <c r="A92" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93" s="1" t="s">
+      <c r="A93" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="94" spans="1:1">
-      <c r="A94" s="1" t="s">
+      <c r="A94" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95" s="1" t="s">
+      <c r="A95" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="96" spans="1:1">
-      <c r="A96" s="1" t="s">
+      <c r="A96" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" s="1" t="s">
+      <c r="A97" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="1" t="s">
+      <c r="A98" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="99" spans="1:1">
-      <c r="A99" s="1" t="s">
+      <c r="A99" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="1" t="s">
+      <c r="A100" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" s="1" t="s">
+      <c r="A101" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="1" t="s">
+      <c r="A102" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="1" t="s">
+      <c r="A103" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="104" spans="1:1">
-      <c r="A104" s="1" t="s">
+      <c r="A104" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="105" spans="1:1">
-      <c r="A105" s="1" t="s">
+      <c r="A105" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="106" spans="1:1">
-      <c r="A106" s="1" t="s">
+      <c r="A106" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="107" spans="1:1">
-      <c r="A107" s="1" t="s">
+      <c r="A107" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="108" spans="1:1">
-      <c r="A108" s="1" t="s">
+      <c r="A108" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="109" spans="1:1">
-      <c r="A109" s="1" t="s">
+      <c r="A109" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="110" spans="1:1">
-      <c r="A110" s="1" t="s">
+      <c r="A110" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="111" spans="1:1">
-      <c r="A111" s="1" t="s">
+      <c r="A111" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="112" spans="1:1">
-      <c r="A112" s="1" t="s">
+      <c r="A112" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="113" spans="1:1">
-      <c r="A113" s="1" t="s">
+      <c r="A113" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="114" spans="1:1">
-      <c r="A114" s="1" t="s">
+      <c r="A114" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="115" spans="1:1">
-      <c r="A115" s="1" t="s">
+      <c r="A115" s="2" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="116" spans="1:1">
-      <c r="A116" s="1" t="s">
+      <c r="A116" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="117" spans="1:1">
-      <c r="A117" s="1" t="s">
+      <c r="A117" s="2" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="118" spans="1:1">
-      <c r="A118" s="1" t="s">
+      <c r="A118" s="2" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="119" spans="1:1">
-      <c r="A119" s="1" t="s">
+      <c r="A119" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="120" spans="1:1">
-      <c r="A120" s="1" t="s">
+      <c r="A120" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="121" spans="1:1">
-      <c r="A121" s="1" t="s">
+      <c r="A121" s="2" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="122" spans="1:1">
-      <c r="A122" s="1" t="s">
+      <c r="A122" s="2" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="123" spans="1:1">
-      <c r="A123" s="1" t="s">
+      <c r="A123" s="2" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="124" spans="1:1">
-      <c r="A124" s="1" t="s">
+      <c r="A124" s="2" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="125" spans="1:1">
-      <c r="A125" s="1" t="s">
+      <c r="A125" s="2" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="126" spans="1:1">
-      <c r="A126" s="1" t="s">
+      <c r="A126" s="2" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="127" spans="1:1">
-      <c r="A127" s="1" t="s">
+      <c r="A127" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="128" spans="1:1">
-      <c r="A128" s="1" t="s">
+      <c r="A128" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="131" spans="1:1">
-      <c r="A131">
+    <row r="131" spans="1:4">
+      <c r="A131" s="1">
         <v>405</v>
       </c>
-    </row>
-    <row r="132" spans="1:1">
-      <c r="A132" s="1" t="s">
+      <c r="C131" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="133" spans="1:1">
-      <c r="A133" s="1" t="s">
+    <row r="133" spans="1:4">
+      <c r="A133" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="134" spans="1:1">
-      <c r="A134" s="1" t="s">
+    <row r="134" spans="1:4">
+      <c r="A134" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="135" spans="1:1">
-      <c r="A135" s="1" t="s">
+    <row r="135" spans="1:4">
+      <c r="A135" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="136" spans="1:1">
-      <c r="A136" s="1" t="s">
+    <row r="136" spans="1:4">
+      <c r="A136" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="137" spans="1:1">
-      <c r="A137" s="1" t="s">
+    <row r="137" spans="1:4">
+      <c r="A137" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
-      <c r="A138" s="1" t="s">
+    <row r="138" spans="1:4">
+      <c r="A138" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="139" spans="1:1">
-      <c r="A139" s="1" t="s">
+    <row r="139" spans="1:4">
+      <c r="A139" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="140" spans="1:1">
-      <c r="A140" s="1" t="s">
+    <row r="140" spans="1:4">
+      <c r="A140" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="141" spans="1:1">
-      <c r="A141" s="1" t="s">
+    <row r="141" spans="1:4">
+      <c r="A141" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="142" spans="1:1">
-      <c r="A142" s="1" t="s">
+    <row r="142" spans="1:4">
+      <c r="A142" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="143" spans="1:1">
-      <c r="A143" s="1" t="s">
+    <row r="143" spans="1:4">
+      <c r="A143" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="144" spans="1:1">
-      <c r="A144" s="1" t="s">
+    <row r="144" spans="1:4">
+      <c r="A144" s="2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="145" spans="1:1">
-      <c r="A145" s="1" t="s">
+      <c r="A145" s="2" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="146" spans="1:1">
-      <c r="A146" s="1" t="s">
+      <c r="A146" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="147" spans="1:1">
-      <c r="A147" s="1" t="s">
+      <c r="A147" s="2" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="148" spans="1:1">
-      <c r="A148" s="1" t="s">
+      <c r="A148" s="2" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="149" spans="1:1">
-      <c r="A149" s="1" t="s">
+      <c r="A149" s="2" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="150" spans="1:1">
-      <c r="A150" s="1" t="s">
+      <c r="A150" s="2" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="151" spans="1:1">
-      <c r="A151" s="1" t="s">
+      <c r="A151" s="2" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="152" spans="1:1">
-      <c r="A152" s="1" t="s">
+      <c r="A152" s="2" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="153" spans="1:1">
-      <c r="A153" s="1" t="s">
+      <c r="A153" s="2" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="154" spans="1:1">
-      <c r="A154" s="1" t="s">
+      <c r="A154" s="2" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="155" spans="1:1">
-      <c r="A155" s="1" t="s">
+      <c r="A155" s="2" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="156" spans="1:1">
-      <c r="A156" s="1" t="s">
+      <c r="A156" s="2" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="157" spans="1:1">
-      <c r="A157" s="1" t="s">
+      <c r="A157" s="2" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="158" spans="1:1">
-      <c r="A158" s="1" t="s">
+      <c r="A158" s="2" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="159" spans="1:1">
-      <c r="A159" s="1" t="s">
+      <c r="A159" s="2" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="160" spans="1:1">
-      <c r="A160" s="1" t="s">
+      <c r="A160" s="2" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="161" spans="1:1">
-      <c r="A161" s="1" t="s">
+      <c r="A161" s="2" t="s">
         <v>137</v>
       </c>
     </row>

</xml_diff>